<commit_message>
Workflow and Issue Filteration module added
</commit_message>
<xml_diff>
--- a/Test Case sumary report.xlsx
+++ b/Test Case sumary report.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="79">
   <si>
     <t>API NAME</t>
   </si>
@@ -184,6 +184,102 @@
   </si>
   <si>
     <t>{'message': 'data format is not right '}</t>
+  </si>
+  <si>
+    <t>IssueIssueByMonth</t>
+  </si>
+  <si>
+    <t>The function of this api is to collect total issue in perticular Month in perticular project</t>
+  </si>
+  <si>
+    <t>TCIBM03</t>
+  </si>
+  <si>
+    <t>TCIBM01</t>
+  </si>
+  <si>
+    <t>TCIBM02</t>
+  </si>
+  <si>
+    <t>get_number_of_issue_by_month_
+api_testing_by_giving_right_parameter</t>
+  </si>
+  <si>
+    <t>get_number_of_issue_by_month_api
+_testing_by_giving_missing_parameter</t>
+  </si>
+  <si>
+    <t>get_number_of_issue_by_month_api
+_testing_by_giving_Wrong_datatype_parameter</t>
+  </si>
+  <si>
+    <t>{"project_id":202}</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>{"project_id":"*&amp;^%$"}</t>
+  </si>
+  <si>
+    <t>{'Issue': 4}</t>
+  </si>
+  <si>
+    <t>{'Error': 'Wrong data type of project id'}</t>
+  </si>
+  <si>
+    <t>IssueIssueByWeek</t>
+  </si>
+  <si>
+    <t>The function of this api is to collect total issue in perticular Week in perticular project</t>
+  </si>
+  <si>
+    <t>TCIBW01</t>
+  </si>
+  <si>
+    <t>TCIBW02</t>
+  </si>
+  <si>
+    <t>TCIBW03</t>
+  </si>
+  <si>
+    <t>get_number_of_issue_by_week_
+api_testing_by_giving_right_parameter</t>
+  </si>
+  <si>
+    <t>get_number_of_issue_by_week_api
+_testing_by_giving_missing_parameter</t>
+  </si>
+  <si>
+    <t>get_number_of_issue_by_week_api
+_testing_by_giving_Wrong_datatype_parameter</t>
+  </si>
+  <si>
+    <t>IssueIssueByQuarter</t>
+  </si>
+  <si>
+    <t>The function of this api is to collect total issue in perticular quarter in perticular project</t>
+  </si>
+  <si>
+    <t>TCIBQ01</t>
+  </si>
+  <si>
+    <t>TCIBQ02</t>
+  </si>
+  <si>
+    <t>TCIBQ03</t>
+  </si>
+  <si>
+    <t>get_number_of_issue_by_Quarter_
+api_testing_by_giving_right_parameter</t>
+  </si>
+  <si>
+    <t>get_number_of_issue_by_Quarter_api
+_testing_by_giving_missing_parameter</t>
+  </si>
+  <si>
+    <t>get_number_of_issue_by_Quarter_api
+_testing_by_giving_Wrong_datatype_parameter</t>
   </si>
 </sst>
 </file>
@@ -609,16 +705,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
@@ -627,8 +723,8 @@
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.140625" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" customWidth="1"/>
+    <col min="11" max="11" width="36.140625" customWidth="1"/>
+    <col min="12" max="12" width="35.7109375" customWidth="1"/>
     <col min="13" max="13" width="25.42578125" customWidth="1"/>
     <col min="14" max="14" width="28" customWidth="1"/>
     <col min="15" max="15" width="26.42578125" customWidth="1"/>
@@ -1095,11 +1191,704 @@
         <v>49</v>
       </c>
     </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="12"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="14"/>
+    </row>
+    <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K53" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L53" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="9">
+        <v>1</v>
+      </c>
+      <c r="E54" s="9">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I54" s="3">
+        <v>200</v>
+      </c>
+      <c r="J54" s="3">
+        <v>200</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="9">
+        <v>1</v>
+      </c>
+      <c r="E55" s="9">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I55" s="3">
+        <v>400</v>
+      </c>
+      <c r="J55" s="3">
+        <v>400</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="9">
+        <v>1</v>
+      </c>
+      <c r="E56" s="9">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I56" s="3">
+        <v>400</v>
+      </c>
+      <c r="J56" s="3">
+        <v>400</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="12"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="13"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="14"/>
+    </row>
+    <row r="63" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="11"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J71" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K71" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L71" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72" s="9">
+        <v>1</v>
+      </c>
+      <c r="E72" s="9">
+        <v>0</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I72" s="3">
+        <v>200</v>
+      </c>
+      <c r="J72" s="3">
+        <v>200</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D73" s="9">
+        <v>1</v>
+      </c>
+      <c r="E73" s="9">
+        <v>0</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I73" s="3">
+        <v>400</v>
+      </c>
+      <c r="J73" s="3">
+        <v>400</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D74" s="9">
+        <v>1</v>
+      </c>
+      <c r="E74" s="9">
+        <v>0</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I74" s="3">
+        <v>400</v>
+      </c>
+      <c r="J74" s="3">
+        <v>400</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L74" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="12"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="13"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B80" s="14"/>
+    </row>
+    <row r="81" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="11"/>
+      <c r="K87" s="11"/>
+      <c r="L87" s="11"/>
+      <c r="M87" s="11"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H89" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I89" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J89" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K89" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L89" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90" s="9">
+        <v>1</v>
+      </c>
+      <c r="E90" s="9">
+        <v>0</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I90" s="3">
+        <v>200</v>
+      </c>
+      <c r="J90" s="3">
+        <v>200</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D91" s="9">
+        <v>1</v>
+      </c>
+      <c r="E91" s="9">
+        <v>0</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I91" s="3">
+        <v>400</v>
+      </c>
+      <c r="J91" s="3">
+        <v>400</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L91" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D92" s="9">
+        <v>1</v>
+      </c>
+      <c r="E92" s="9">
+        <v>0</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I92" s="3">
+        <v>400</v>
+      </c>
+      <c r="J92" s="3">
+        <v>400</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="20">
+    <mergeCell ref="A69:M69"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A87:M87"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A51:M51"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A42:B42"/>
     <mergeCell ref="A12:M12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>

</xml_diff>